<commit_message>
codes for read configure
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -6041,8 +6041,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -7147,7 +7147,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -7774,7 +7774,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>